<commit_message>
CD3 Changes - moved Oracle-Tags from example to after <END>, San Jose to SanJose in Excel drop down, Renamed DRGv2 to CIS, Changed Instance example, Added NLB sheets.
</commit_message>
<xml_diff>
--- a/oci_tools/cd3_automation_toolkit/example/CD3-ManagementServices-template.xlsx
+++ b/oci_tools/cd3_automation_toolkit/example/CD3-ManagementServices-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shrsubra/Desktop/Shruthi/cd3-automation/oci/oci_tools/cd3_automation_toolkit/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D268D5C-A6BD-D240-8C76-D97666CDA64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FC124C-19A2-0E48-B5A1-437E1E857170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23000" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3665,7 +3665,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>CD3 Automation Toolkit Release - v9.1</t>
+      <t>CD3 Automation Toolkit Release - v9.2</t>
     </r>
   </si>
 </sst>

</xml_diff>